<commit_message>
Fix serious backstab/sneak bug
- Character would continue backstabbing after dead.

Now sneak status is removed whenever the character cannot move
either from death or a status like sleep or numb
</commit_message>
<xml_diff>
--- a/dev/steal.xlsx
+++ b/dev/steal.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{066DA4DE-C347-490E-83C2-A9C599B6EAF4}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{669B205E-8587-49A1-8165-6BE91E9B6C03}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="237">
   <si>
     <t>Id</t>
   </si>
@@ -728,6 +728,9 @@
   </si>
   <si>
     <t>Chi-Kunai</t>
+  </si>
+  <si>
+    <t>Joint</t>
   </si>
 </sst>
 </file>
@@ -1048,8 +1051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:D206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1329,7 +1332,7 @@
         <v>25</v>
       </c>
       <c r="C24" t="s">
-        <v>170</v>
+        <v>236</v>
       </c>
       <c r="D24" s="1">
         <v>0.5</v>

</xml_diff>